<commit_message>
new script and object repos committed
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerModules.xlsx
+++ b/src/test/resources/VtigerModules.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Predator\Vtiger_Automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAKSHMAN BABU THOTA\git\VtigerNewFW\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA151156-0D83-4170-A5BB-42C14B0A95EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C1E808E-2783-49F9-8E39-2AF4C430FF06}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Opportunity" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Opportunity_Name</t>
   </si>
@@ -40,12 +39,41 @@
   </si>
   <si>
     <t>pradeep</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Assigned_To</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Ross Taylor</t>
+  </si>
+  <si>
+    <t>Value Proposition</t>
+  </si>
+  <si>
+    <t>Support Group</t>
+  </si>
+  <si>
+    <t>Ross Taylor is kiwi business man. 
+He is investing his money in the 
+new business.</t>
+  </si>
+  <si>
+    <t>Organisation_Name</t>
+  </si>
+  <si>
+    <t>Kiwi organisations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,11 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,21 +445,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9804AACC-231F-400E-A8EC-E1608BB5D1CE}">
-  <dimension ref="A2:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -448,6 +482,46 @@
       </c>
       <c r="C3" s="3">
         <v>45066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>500</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>